<commit_message>
Ejecucion Scaffold new bd rcapp2
</commit_message>
<xml_diff>
--- a/BD/DiagramaActividades.xlsx
+++ b/BD/DiagramaActividades.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FullStack\reciclapp\BD\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="9630" firstSheet="1" activeTab="2"/>
   </bookViews>
@@ -20,7 +15,7 @@
     <sheet name="PLANILLASREPORTE" sheetId="7" r:id="rId6"/>
     <sheet name="USUARIO" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="241">
   <si>
     <t>N° Actividad</t>
   </si>
@@ -89,9 +84,6 @@
     <t>PUNTACION</t>
   </si>
   <si>
-    <t>USUARIOS</t>
-  </si>
-  <si>
     <t>idusuario</t>
   </si>
   <si>
@@ -347,9 +339,6 @@
     <t>idpuntoecologico</t>
   </si>
   <si>
-    <t>Ubicación</t>
-  </si>
-  <si>
     <t>Idretousuario</t>
   </si>
   <si>
@@ -623,9 +612,6 @@
     <t>idrecoleccion</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>celular</t>
   </si>
   <si>
@@ -662,16 +648,112 @@
     <t xml:space="preserve">:datetime </t>
   </si>
   <si>
-    <t xml:space="preserve">rails generate scaffold usuario </t>
-  </si>
-  <si>
     <t>rails generate scaffold usuario idusuario:integer nombre:string apellido:string celular:string email:string fechanacimiento:datetime direccion:string barrio:string edificio:string genero:string empresa:string clienteacueducto:string jac:string idperfildetpar:integer idlocalidad:integer  --force</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rails generate scaffold </t>
+  </si>
+  <si>
+    <t xml:space="preserve">usuario </t>
+  </si>
+  <si>
+    <t xml:space="preserve">parametro </t>
+  </si>
+  <si>
+    <t xml:space="preserve">detalleparametro </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rails generate scaffold parametro idparametro:integer nombre:string </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rails generate scaffold detalleparametro iddetalleparametro:integer idparametro:integer nombre:string </t>
+  </si>
+  <si>
+    <t>lema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">retousuario </t>
+  </si>
+  <si>
+    <t>idusuario_origina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rails generate scaffold reto Idreto:integer idusuario_origina:integer nombre:string </t>
+  </si>
+  <si>
+    <t xml:space="preserve">recoleccion </t>
+  </si>
+  <si>
+    <t>META</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rails generate scaffold meta Idmeta:integer idusuario:integer iddetalleparametro:integer idreto:integer Fechaexpiracion:datetime cantidad:integer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">redencion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">puntoecologico </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rails generate scaffold redencion idredencion:integer idusuario:integer idpremio:integer fecharedencion:datetime Cantidadpremio:integer </t>
+  </si>
+  <si>
+    <t>idventas</t>
+  </si>
+  <si>
+    <t>fechaventa</t>
+  </si>
+  <si>
+    <t>valor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">venta </t>
+  </si>
+  <si>
+    <t>USUARIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rails generate scaffold retousuario idreto:integer idusu_invitado:integer lema:integer </t>
+  </si>
+  <si>
+    <t>Idreto (fk)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rails generate scaffold recoleccion idrecoleccion:integer Idretousuario:integer idusu_invitado:integer iddetalleparametro:integer idredencion:integer idpuntorecoleccion:integer Estado:string Fecha:datetime Cantidad:integer </t>
+  </si>
+  <si>
+    <t>Ubicacionx</t>
+  </si>
+  <si>
+    <t>Ubicaciony</t>
+  </si>
+  <si>
+    <t>rails g scaffold list name</t>
+  </si>
+  <si>
+    <t>rails g scaffold task name list:references</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:decimal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rails generate scaffold puntoecologico idpuntoecologico:integer Ubicacionx:decimal Ubicaciony:decimal Nombre:string idresponsable:integer Fechainicio:datetime Fechacierre:datetime </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rails generate scaffold venta idventas:integer idpuntoecologico:integer iddetalleparametro:integer fechaventa:datetime cantidad:integer valor:integer donacion:string </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -717,7 +799,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -739,6 +821,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,7 +896,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -842,6 +930,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -911,15 +1000,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>109714</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>45178</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>149954</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -942,8 +1031,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1123950" y="1419225"/>
-          <a:ext cx="10058400" cy="6436453"/>
+          <a:off x="1133475" y="2586214"/>
+          <a:ext cx="9886950" cy="6326740"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1210,7 +1299,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1734,56 +1823,56 @@
       <c r="B15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="20"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>1</v>
       </c>
       <c r="B16" s="9"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>2</v>
       </c>
       <c r="B17" s="9"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="17"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="18"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>3</v>
       </c>
       <c r="B18" s="9"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="17"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="18"/>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
@@ -1855,7 +1944,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="I2" sqref="I2:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,18 +1952,19 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>230</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
@@ -1883,33 +1973,33 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E1" t="s">
-        <v>62</v>
+        <v>100</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
+        <v>193</v>
       </c>
       <c r="G1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>66</v>
+        <v>220</v>
+      </c>
+      <c r="H1" t="s">
+        <v>74</v>
       </c>
       <c r="I1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K1" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -1918,309 +2008,677 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
-        <v>90</v>
+        <v>194</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="I2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" t="s">
         <v>106</v>
       </c>
-      <c r="J2" t="s">
-        <v>104</v>
-      </c>
       <c r="K2" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>162</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>216</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>67</v>
+        <v>234</v>
       </c>
       <c r="J3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K3" t="s">
-        <v>104</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>90</v>
       </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
       <c r="I4" t="s">
-        <v>164</v>
+        <v>235</v>
       </c>
       <c r="J4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" t="s">
-        <v>92</v>
+      <c r="G5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" t="s">
+        <v>91</v>
       </c>
       <c r="I5" t="s">
-        <v>165</v>
+        <v>15</v>
       </c>
       <c r="J5" t="s">
-        <v>187</v>
-      </c>
-      <c r="K5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>193</v>
-      </c>
-      <c r="D6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
+        <v>191</v>
       </c>
       <c r="F6" t="s">
-        <v>93</v>
+        <v>89</v>
+      </c>
+      <c r="G6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" t="s">
+        <v>185</v>
       </c>
       <c r="J6" t="s">
-        <v>169</v>
-      </c>
-      <c r="K6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" t="s">
-        <v>65</v>
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" t="s">
+        <v>167</v>
       </c>
       <c r="J7" t="s">
-        <v>170</v>
-      </c>
-      <c r="K7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>194</v>
-      </c>
-      <c r="D8" t="s">
-        <v>102</v>
-      </c>
-      <c r="K8" t="s">
-        <v>111</v>
+        <v>192</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" t="s">
+        <v>168</v>
+      </c>
+      <c r="J8" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" t="s">
-        <v>57</v>
+        <v>96</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" t="s">
-        <v>56</v>
+        <v>97</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="3.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D3" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="H3" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="E1" t="s">
-        <v>193</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I3" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J3" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K3" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L3" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M3" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="O3" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="K1" t="s">
-        <v>204</v>
-      </c>
-      <c r="L1" t="s">
-        <v>205</v>
-      </c>
-      <c r="M1" t="s">
-        <v>96</v>
-      </c>
-      <c r="N1" t="s">
-        <v>186</v>
-      </c>
-      <c r="O1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>210</v>
-      </c>
-      <c r="D3" t="str">
-        <f>CONCATENATE(A3,A1,A5,B1,A4,C1,A4,D1,A4,E1,A4,F1,A6,G1,A4,H1,A4,I1,A4,J1,A4,K1,A4,L1,A4,M1,A4,N1,A5,O1,A5," --force")</f>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>CONCATENATE(F1,A2,A3,B1,B3,A1,C3,A1,D3,A1,E3,A1,F3,C1,G3,A1,H3,A1,I3,A1,J3,A1,K3,A1,L3,A1,M3,A1,N3,B1,O3,B1," --force")</f>
         <v>rails generate scaffold usuario idusuario:integer nombre:string apellido:string celular:string email:string fechanacimiento:datetime direccion:string barrio:string edificio:string genero:string empresa:string clienteacueducto:string jac:string idperfildetpar:integer idlocalidad:integer  --force</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="B8" s="15"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>CONCATENATE($F$1,A8,A9,B1,B9,A1)</f>
+        <v xml:space="preserve">rails generate scaffold parametro idparametro:integer nombre:string </v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>CONCATENATE($F$1,A15,A16,B1,B16,B1,C16,A1)</f>
+        <v xml:space="preserve">rails generate scaffold detalleparametro iddetalleparametro:integer idparametro:integer nombre:string </v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>CONCATENATE($F$1,A22,A23,B1,B23,B1,C23,B1)</f>
+        <v xml:space="preserve">rails generate scaffold retousuario idreto:integer idusu_invitado:integer lema:integer </v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>CONCATENATE($F$1,A29,A30,$B$1,B30,$B$1,C30,$A$1)</f>
+        <v xml:space="preserve">rails generate scaffold reto Idreto:integer idusuario_origina:integer nombre:string </v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I37" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37" s="15"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f>CONCATENATE($F$1,A36,A37,$B$1,B37,$B$1,C37,$B$1,D37,B1,E37,B1,F37,B1,G37,A1,H37,C1,I37,B1)</f>
+        <v xml:space="preserve">rails generate scaffold recoleccion idrecoleccion:integer Idretousuario:integer idusu_invitado:integer iddetalleparametro:integer idredencion:integer idpuntorecoleccion:integer Estado:string Fecha:datetime Cantidad:integer </v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
+        <f>CONCATENATE($F$1,A43,A44,$B$1,B44,$B$1,C44,$B$1,D44,B1,E44,C1,F44,B1)</f>
+        <v xml:space="preserve">rails generate scaffold meta Idmeta:integer idusuario:integer iddetalleparametro:integer idreto:integer Fechaexpiracion:datetime cantidad:integer </v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="str">
+        <f>CONCATENATE($F$1,A50,A51,$B$1,B51,$B$1,C51,$B$1,D51,$C$1,E51,$B$1)</f>
+        <v xml:space="preserve">rails generate scaffold redencion idredencion:integer idusuario:integer idpremio:integer fecharedencion:datetime Cantidadpremio:integer </v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G57" s="15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="str">
+        <f>CONCATENATE($F$1,A56,A57,$B$1,B57,$D$1,C57,$D$1,D57,$A$1,E57,$B$1,F57,C1,G57,C1)</f>
+        <v xml:space="preserve">rails generate scaffold puntoecologico idpuntoecologico:integer Ubicacionx:decimal Ubicaciony:decimal Nombre:string idresponsable:integer Fechainicio:datetime Fechacierre:datetime </v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F64" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="G64" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="str">
+        <f>CONCATENATE($F$1,A63,A64,$B$1,B64,$B$1,C64,$B$1,D64,$C$1,E64,$B$1,F64,$B$1,G64,$A$1)</f>
+        <v xml:space="preserve">rails generate scaffold venta idventas:integer idpuntoecologico:integer iddetalleparametro:integer fechaventa:datetime cantidad:integer valor:integer donacion:string </v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2246,7 +2704,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
@@ -2266,7 +2724,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2275,20 +2733,20 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M2" t="str">
         <f>CONCATENATE(K2,H2,",",I2,",'",J2,"'),")</f>
         <v>(1,1,'Aceite'),</v>
       </c>
       <c r="N2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -2299,20 +2757,20 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M3" t="str">
         <f>CONCATENATE(K3,H3,",",I3,",'",J3,"'),")</f>
         <v>(2,1,'Medicamentos'),</v>
       </c>
       <c r="N3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2323,20 +2781,20 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K4" t="s">
+        <v>115</v>
+      </c>
+      <c r="L4" s="13" t="s">
         <v>114</v>
-      </c>
-      <c r="K4" t="s">
-        <v>117</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>116</v>
       </c>
       <c r="M4" t="str">
         <f>CONCATENATE(K4,H4,",",I4,",'",J4,"'),")</f>
         <v>(3,1,'Metal'),</v>
       </c>
       <c r="N4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -2347,20 +2805,20 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" ref="M5:M34" si="0">CONCATENATE(K5,H5,",",I5,",'",J5,"'),")</f>
         <v>(4,1,'Papel'),</v>
       </c>
       <c r="N5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -2371,20 +2829,20 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
         <v>(5,1,'Plastico'),</v>
       </c>
       <c r="N6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -2395,20 +2853,20 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
         <v>(6,1,'Tecnologico'),</v>
       </c>
       <c r="N7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -2419,20 +2877,20 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
         <v>(7,1,'Telas'),</v>
       </c>
       <c r="N8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -2440,7 +2898,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9">
         <v>8</v>
@@ -2449,20 +2907,20 @@
         <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="0"/>
         <v>(8,2,'Usaquén'),</v>
       </c>
       <c r="N9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -2473,20 +2931,20 @@
         <v>2</v>
       </c>
       <c r="J10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="0"/>
         <v>(9,2,'Chapinero'),</v>
       </c>
       <c r="N10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -2497,20 +2955,20 @@
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="0"/>
         <v>(10,2,'Santa Fe'),</v>
       </c>
       <c r="N11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -2521,20 +2979,20 @@
         <v>2</v>
       </c>
       <c r="J12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="0"/>
         <v>(11,2,'San Cristóbal'),</v>
       </c>
       <c r="N12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -2545,20 +3003,20 @@
         <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="0"/>
         <v>(12,2,'Usme'),</v>
       </c>
       <c r="N13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2569,20 +3027,20 @@
         <v>2</v>
       </c>
       <c r="J14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="0"/>
         <v>(13,2,'Tunjuelito'),</v>
       </c>
       <c r="N14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2593,20 +3051,20 @@
         <v>2</v>
       </c>
       <c r="J15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="0"/>
         <v>(14,2,'Bosa'),</v>
       </c>
       <c r="N15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2617,20 +3075,20 @@
         <v>2</v>
       </c>
       <c r="J16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="0"/>
         <v>(15,2,'Kennedy'),</v>
       </c>
       <c r="N16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -2641,20 +3099,20 @@
         <v>2</v>
       </c>
       <c r="J17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="0"/>
         <v>(16,2,'Fontibón'),</v>
       </c>
       <c r="N17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -2665,20 +3123,20 @@
         <v>2</v>
       </c>
       <c r="J18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="0"/>
         <v>(17,2,'Engativá'),</v>
       </c>
       <c r="N18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -2689,20 +3147,20 @@
         <v>2</v>
       </c>
       <c r="J19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="0"/>
         <v>(18,2,'Suba'),</v>
       </c>
       <c r="N19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -2713,20 +3171,20 @@
         <v>2</v>
       </c>
       <c r="J20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L20" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="0"/>
         <v>(19,2,'Barrios Unidos'),</v>
       </c>
       <c r="N20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -2737,20 +3195,20 @@
         <v>2</v>
       </c>
       <c r="J21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L21" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="0"/>
         <v>(20,2,'Teusaquillo'),</v>
       </c>
       <c r="N21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -2761,20 +3219,20 @@
         <v>2</v>
       </c>
       <c r="J22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L22" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="0"/>
         <v>(21,2,'Los Mártires'),</v>
       </c>
       <c r="N22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -2785,20 +3243,20 @@
         <v>2</v>
       </c>
       <c r="J23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L23" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="0"/>
         <v>(22,2,'Antonio Nariño'),</v>
       </c>
       <c r="N23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -2809,20 +3267,20 @@
         <v>2</v>
       </c>
       <c r="J24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L24" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="0"/>
         <v>(23,2,'Puente Aranda'),</v>
       </c>
       <c r="N24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -2833,20 +3291,20 @@
         <v>2</v>
       </c>
       <c r="J25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="0"/>
         <v>(24,2,'La Candelaria'),</v>
       </c>
       <c r="N25" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -2857,20 +3315,20 @@
         <v>2</v>
       </c>
       <c r="J26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L26" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="0"/>
         <v>(25,2,'Rafael Uribe Uribe'),</v>
       </c>
       <c r="N26" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -2881,20 +3339,20 @@
         <v>2</v>
       </c>
       <c r="J27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L27" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="0"/>
         <v>(26,2,'Ciudad Bolívar'),</v>
       </c>
       <c r="N27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -2905,20 +3363,20 @@
         <v>2</v>
       </c>
       <c r="J28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L28" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="0"/>
         <v>(27,2,'Sumapaz'),</v>
       </c>
       <c r="N28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -2926,7 +3384,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H29">
         <v>28</v>
@@ -2935,20 +3393,20 @@
         <v>3</v>
       </c>
       <c r="J29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L29" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="0"/>
         <v>(28,3,'Pendiente'),</v>
       </c>
       <c r="N29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -2959,20 +3417,20 @@
         <v>3</v>
       </c>
       <c r="J30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K30" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="0"/>
         <v>(29,3,'Redimido'),</v>
       </c>
       <c r="N30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -2980,7 +3438,7 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H31">
         <v>30</v>
@@ -2989,20 +3447,20 @@
         <v>4</v>
       </c>
       <c r="J31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L31" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" si="0"/>
         <v>(30,4,'Boletas Cine'),</v>
       </c>
       <c r="N31" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -3013,20 +3471,20 @@
         <v>4</v>
       </c>
       <c r="J32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L32" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M32" t="str">
         <f t="shared" si="0"/>
         <v>(31,4,'Boletas Maloka'),</v>
       </c>
       <c r="N32" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -3037,20 +3495,20 @@
         <v>4</v>
       </c>
       <c r="J33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L33" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" si="0"/>
         <v>(32,4,'Dto 25%'),</v>
       </c>
       <c r="N33" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -3061,20 +3519,20 @@
         <v>4</v>
       </c>
       <c r="J34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K34" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L34" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" si="0"/>
         <v>(33,4,'Dto 20%'),</v>
       </c>
       <c r="N34" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -3085,20 +3543,20 @@
         <v>4</v>
       </c>
       <c r="J35" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K35" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L35" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M35" t="str">
         <f>CONCATENATE(K35,H35,",",I35,",'",J35,"'),")</f>
         <v>(34,4,'Ganancia Recoleccion'),</v>
       </c>
       <c r="N35" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -3106,7 +3564,7 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H36">
         <v>35</v>
@@ -3115,20 +3573,20 @@
         <v>5</v>
       </c>
       <c r="J36" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K36" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L36" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M36" t="str">
         <f>CONCATENATE(K36,H36,",",I36,",'",J36,"'),")</f>
         <v>(35,5,'Administrador'),</v>
       </c>
       <c r="N36" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -3139,20 +3597,20 @@
         <v>5</v>
       </c>
       <c r="J37" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L37" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M37" t="str">
         <f>CONCATENATE(K37,H37,",",I37,",'",J37,"'),")</f>
         <v>(36,5,'Responsalbe'),</v>
       </c>
       <c r="N37" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -3163,20 +3621,20 @@
         <v>5</v>
       </c>
       <c r="J38" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K38" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L38" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M38" t="str">
         <f>CONCATENATE(K38,H38,",",I38,",'",J38,"'),")</f>
         <v>(37,5,'Voluntario'),</v>
       </c>
       <c r="N38" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -3187,20 +3645,20 @@
         <v>5</v>
       </c>
       <c r="J39" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K39" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L39" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M39" t="str">
         <f>CONCATENATE(K39,H39,",",I39,",'",J39,"'),")</f>
         <v>(38,5,'Usuario'),</v>
       </c>
       <c r="N39" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3223,7 +3681,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3231,45 +3689,45 @@
         <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
       </c>
       <c r="K3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" t="s">
         <v>64</v>
-      </c>
-      <c r="M3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -3289,7 +3747,7 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -3324,7 +3782,7 @@
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -3344,18 +3802,18 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H11" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" t="s">
         <v>66</v>
       </c>
-      <c r="I11" t="s">
-        <v>67</v>
-      </c>
       <c r="J11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K11" t="s">
         <v>15</v>
@@ -3369,29 +3827,29 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -3403,7 +3861,7 @@
         <v>2</v>
       </c>
       <c r="L19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -3417,7 +3875,7 @@
         <v>3</v>
       </c>
       <c r="L20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -3431,7 +3889,7 @@
         <v>4</v>
       </c>
       <c r="L21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3456,13 +3914,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -3476,7 +3934,7 @@
         <v>43379</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3490,7 +3948,7 @@
         <v>43379</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3504,7 +3962,7 @@
         <v>43379</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -3518,7 +3976,7 @@
         <v>43379</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -3532,7 +3990,7 @@
         <v>43379</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -3546,7 +4004,7 @@
         <v>43379</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -3560,7 +4018,7 @@
         <v>43379</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -3575,7 +4033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T7"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -3596,49 +4054,49 @@
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
+      <c r="L2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J2" t="s">
-        <v>99</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>115</v>
-      </c>
-      <c r="M2" t="s">
-        <v>28</v>
-      </c>
       <c r="N2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -3646,31 +4104,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
         <v>77</v>
-      </c>
-      <c r="C3" t="s">
-        <v>78</v>
       </c>
       <c r="D3">
         <v>319360</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F3" s="11">
         <v>31507</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I3" t="s">
         <v>153</v>
       </c>
-      <c r="I3" t="s">
-        <v>155</v>
-      </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L3" t="str">
         <f>CONCATENATE(B3," ",C3)</f>
@@ -3680,26 +4138,26 @@
         <v>456879</v>
       </c>
       <c r="N3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="O3">
         <v>35</v>
       </c>
       <c r="P3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Q3" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R3" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S3" t="str">
         <f>CONCATENATE(P3,A3,",",Q3,B3,R3,C3,R3,D3,R3,,E3,R3,F3,R3,G3,R3,H3,R3,I3,R3,J3,R3,K3,R3,L3,R3,M3,R3,N3,R3,O3,"'),")</f>
         <v>(1,'NIKOLAY','CARDENAS','319360','nikolay37@hotmail.com','31507','Suba','Calle 136','Costa Azul','','M','NIKOLAY CARDENAS','456879','Costa Azul','35'),</v>
       </c>
       <c r="T3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -3707,28 +4165,28 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
         <v>80</v>
-      </c>
-      <c r="C4" t="s">
-        <v>81</v>
       </c>
       <c r="D4">
         <v>319360</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F4" s="11">
         <v>31507</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L4" t="str">
         <f>CONCATENATE(B4," ",C4)</f>
@@ -3738,26 +4196,26 @@
         <v>654987</v>
       </c>
       <c r="N4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="O4">
         <v>35</v>
       </c>
       <c r="P4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Q4" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R4" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S4" t="str">
         <f>CONCATENATE(P4,A4,",",Q4,B4,R4,C4,R4,D4,R4,,E4,R4,F4,R4,G4,R4,H4,R4,I4,R4,J4,R4,K4,R4,L4,R4,M4,R4,N4,R4,O4,"'),")</f>
         <v>(2,'JULIAN','RESTREPO','319360','julianrd19@hotmail.com','31507','Suba','Calle 138','','','M','JULIAN RESTREPO','654987','Costa Azul I','35'),</v>
       </c>
       <c r="T4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -3765,28 +4223,28 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
         <v>82</v>
-      </c>
-      <c r="C5" t="s">
-        <v>83</v>
       </c>
       <c r="D5">
         <v>319360</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F5" s="11">
         <v>31507</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L5" t="str">
         <f>CONCATENATE(B5," ",C5)</f>
@@ -3796,26 +4254,26 @@
         <v>753159</v>
       </c>
       <c r="N5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O5">
         <v>35</v>
       </c>
       <c r="P5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Q5" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R5" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S5" t="str">
         <f>CONCATENATE(P5,A5,",",Q5,B5,R5,C5,R5,D5,R5,,E5,R5,F5,R5,G5,R5,H5,R5,I5,R5,J5,R5,K5,R5,L5,R5,M5,R5,N5,R5,O5,"'),")</f>
         <v>(3,'ANDRES','MORENO','319360','andresmorenopinzon@gmail.com','31507','Suba','Calle 140','','','M','ANDRES MORENO','753159','jac 1','35'),</v>
       </c>
       <c r="T5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -3823,28 +4281,28 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" t="s">
         <v>85</v>
-      </c>
-      <c r="C6" t="s">
-        <v>86</v>
       </c>
       <c r="D6">
         <v>3178140952</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F6" s="11">
         <v>31507</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L6" t="str">
         <f>CONCATENATE(B6," ",C6)</f>
@@ -3854,26 +4312,26 @@
         <v>258147</v>
       </c>
       <c r="N6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O6">
         <v>38</v>
       </c>
       <c r="P6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Q6" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R6" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S6" t="str">
         <f>CONCATENATE(P6,A6,",",Q6,B6,R6,C6,R6,D6,R6,,E6,R6,F6,R6,G6,R6,H6,R6,I6,R6,J6,R6,K6,R6,L6,R6,M6,R6,N6,R6,O6,"'),")</f>
         <v>(4,'DIEGO','MENA','3178140952','ingelectronicadj@gmail.com','31507','Suba','Calle 142','','','M','DIEGO MENA','258147','jac 1','38'),</v>
       </c>
       <c r="T6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -3881,31 +4339,31 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D7">
         <v>3143815824</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F7" s="11">
         <v>31507</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L7" t="str">
         <f>CONCATENATE(B7," ",C7)</f>
@@ -3915,26 +4373,26 @@
         <v>258147</v>
       </c>
       <c r="N7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O7">
         <v>38</v>
       </c>
       <c r="P7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Q7" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R7" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S7" t="str">
         <f>CONCATENATE(P7,A7,",",Q7,B7,R7,C7,R7,D7,R7,,E7,R7,F7,R7,G7,R7,H7,R7,I7,R7,J7,R7,K7,R7,L7,R7,M7,R7,N7,R7,O7,"'),")</f>
         <v>(5,'NATALIA','ORTIZ','3143815824','nataliaortiz@gmail.com','31507','Suba','Calle 144','','Las Brisas','F','NATALIA ORTIZ','258147','jac 3','38'),</v>
       </c>
       <c r="T7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -3946,6 +4404,5 @@
     <hyperlink ref="E7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rails con references FK
</commit_message>
<xml_diff>
--- a/BD/DiagramaActividades.xlsx
+++ b/BD/DiagramaActividades.xlsx
@@ -9,12 +9,13 @@
   <sheets>
     <sheet name="Gráfico" sheetId="2" r:id="rId1"/>
     <sheet name="BD" sheetId="3" r:id="rId2"/>
-    <sheet name="Scaffold (Rails)" sheetId="10" r:id="rId3"/>
-    <sheet name="Scaffold" sheetId="9" r:id="rId4"/>
-    <sheet name="PARAMETROS" sheetId="4" r:id="rId5"/>
-    <sheet name="PUNTUACION" sheetId="6" r:id="rId6"/>
-    <sheet name="PLANILLASREPORTE" sheetId="7" r:id="rId7"/>
-    <sheet name="USUARIO" sheetId="8" r:id="rId8"/>
+    <sheet name="Scaffold (Rails) (FK)" sheetId="11" r:id="rId3"/>
+    <sheet name="Scaffold (Rails)" sheetId="10" r:id="rId4"/>
+    <sheet name="Scaffold" sheetId="9" r:id="rId5"/>
+    <sheet name="PARAMETROS" sheetId="4" r:id="rId6"/>
+    <sheet name="PUNTUACION" sheetId="6" r:id="rId7"/>
+    <sheet name="PLANILLASREPORTE" sheetId="7" r:id="rId8"/>
+    <sheet name="USUARIO" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="270">
   <si>
     <t>N° Actividad</t>
   </si>
@@ -803,6 +804,39 @@
   </si>
   <si>
     <t xml:space="preserve">rails generate scaffold venta iddetalleparametro:integer idredencion:integer fechaventa:datetime cantidad:integer valorunidad:integer total:integer donacion:string </t>
+  </si>
+  <si>
+    <t>reto:references usuario:references</t>
+  </si>
+  <si>
+    <t>reto:references reto:detalleparametro</t>
+  </si>
+  <si>
+    <t>reto:retousuario reto:detalleparametro</t>
+  </si>
+  <si>
+    <t>idventa</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>rails generate scaffold retousuario lema:string reto:references users:references</t>
+  </si>
+  <si>
+    <t>fechaexpiracion</t>
+  </si>
+  <si>
+    <t>rails generate scaffold meta fechaexpiracion:datetime cantidad:integer retos:references detalleparametros:references</t>
+  </si>
+  <si>
+    <t>rails generate scaffold recoleccion idusu_invitado:integer iddetalleparametro:integer idredencion:integer idpuntorecoleccion:integer estado:string fecha:datetime cantidad:integer idventa:integer retousuario:references detalleparametro:references</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recoleccions </t>
+  </si>
+  <si>
+    <t>rails generate scaffold redencion idusuario:integer idpremio:integer fecharedencion:integer Cantidadpremio:datetime Cantidadpremio:integer reto:references</t>
   </si>
 </sst>
 </file>
@@ -1355,7 +1389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2284,8 +2318,8 @@
   <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F57" sqref="F57"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2313,7 +2347,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>209</v>
+        <v>263</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -2380,6 +2414,425 @@
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>CONCATENATE(F1,A2,A3,A1,B3,A1,C3,A1,D3,A1,E3,A1,F3,C1,G3,A1,H3,A1,I3,A1,J3,A1,K3,A1,L3,A1,M3,A1,N3,B1,O3,B1," --force")</f>
+        <v>rails generate scaffold userscedula:string nombre:string apellido:string celular:string email:string fechanacimiento:datetime direccion:string barrio:string edificio:string genero:string empresa:string clienteacueducto:string jac:string idperfildetpar:integer idlocalidad:integer  --force</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" s="15"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>CONCATENATE($F$1,A9,A10,$B$1,B10,$A$1)</f>
+        <v xml:space="preserve">rails generate scaffold reto idusuario_origina:integer nombre:string </v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B15" s="15"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>CONCATENATE($F$1,A15,A16,A1)</f>
+        <v xml:space="preserve">rails generate scaffold retousuario lema:string </v>
+      </c>
+      <c r="F18" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="B21" s="15"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>CONCATENATE($F$1,A21,A22,$C$1,B22,$B$1)</f>
+        <v xml:space="preserve">rails generate scaffold meta fechaexpiracion:datetime cantidad:integer </v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="J28" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f>CONCATENATE($F$1,A27,A28,$B$1,B28,$B$1,C28,$B$1,D28,B1,E28,A1,F28,C1,G28,B1,H28,B1)</f>
+        <v xml:space="preserve">rails generate scaffold recoleccions idusu_invitado:integer iddetalleparametro:integer idredencion:integer idpuntorecoleccion:integer estado:string fecha:datetime cantidad:integer idventa:integer </v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f>CONCATENATE($F$1,A33,A34,$B$1,B34,$B$1,C34,$B$1,D34,$C$1,E34,$B$1)</f>
+        <v xml:space="preserve">rails generate scaffold redencion idusuario:integer idpremio:integer fecharedencion:integer Cantidadpremio:datetime Cantidadpremio:integer </v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f>CONCATENATE($F$1,A39,A40,$D$1,B40,$D$1,C40,$A$1,D40,$A$1,E40,$C$1,F40,C1)</f>
+        <v xml:space="preserve">rails generate scaffold puntoecologico ubicacionx:decimal ubicaciony:decimal nombre:string idresponsable:string fechainicio:datetime fechacierre:datetime </v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="G47" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="str">
+        <f>CONCATENATE($F$1,A46,A47,$B$1,B47,$B$1,C47,$C$1,D47,$B$1,E47,$B$1,F47,$B$1,G47,A1)</f>
+        <v xml:space="preserve">rails generate scaffold venta iddetalleparametro:integer idredencion:integer fechaventa:datetime cantidad:integer valorunidad:integer total:integer donacion:string </v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="str">
+        <f>CONCATENATE($F$1,A53,A54,B1)</f>
+        <v xml:space="preserve">rails generate scaffold parametro nombre:integer </v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="15"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="str">
+        <f>CONCATENATE($F$1,A60,A61,B1,B61,A1)</f>
+        <v xml:space="preserve">rails generate scaffold detalleparametro idparametro:integer nombre:string </v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="3.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>CONCATENATE(F1,A2,A3,A1,B3,A1,C3,A1,D3,A1,E3,A1,F3,C1,G3,A1,H3,A1,I3,A1,J3,A1,K3,A1,L3,A1,M3,A1,N3,B1,O3,B1," --force")</f>
         <v>rails generate scaffold usuario cedula:string nombre:string apellido:string celular:string email:string fechanacimiento:datetime direccion:string barrio:string edificio:string genero:string empresa:string clienteacueducto:string jac:string idperfildetpar:integer idlocalidad:integer  --force</v>
       </c>
     </row>
@@ -2704,7 +3157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O70"/>
   <sheetViews>
@@ -3163,7 +3616,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N39"/>
   <sheetViews>
@@ -4147,7 +4600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M21"/>
   <sheetViews>
@@ -4378,7 +4831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -4510,7 +4963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T7"/>
   <sheetViews>

</xml_diff>